<commit_message>
Tested and pushing latest Dispatcher.
</commit_message>
<xml_diff>
--- a/Anagha_Rajendran/customerTransaction/Data/Input/Transanctions.xlsx
+++ b/Anagha_Rajendran/customerTransaction/Data/Input/Transanctions.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JuniorsCode\Customer_Transactions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anagha.n\Documents\UiPath\Github_2023March\Anagha_Rajendran\customerTransaction\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E23B42-039D-4E09-B916-5B19DD981344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F87CFB-83FD-42FA-B336-9EABA23CF6EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A4097C6F-31AD-4BA8-A8BD-AB3096DBD90F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{A4097C6F-31AD-4BA8-A8BD-AB3096DBD90F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -437,7 +426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69EC9DF7-15F1-4F97-A115-E18FF12014E0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1028C7A6-9253-4DFD-AC4B-67B45F3D3145}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>